<commit_message>
Mejora nombres de recursos
Se diferencian más los nombres
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion07/ESCALETA_CN_08_07_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion07/ESCALETA_CN_08_07_CO.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="226">
   <si>
     <t>Asignatura</t>
   </si>
@@ -428,12 +428,6 @@
     <t>Interactivo que trata sobre mutaciones y enfermedades genéticas</t>
   </si>
   <si>
-    <t xml:space="preserve">Primera imagen del menú es tipos de mutación, que lleva las imágenes de mutación: somática, germinal, génica, cromosómica, genómica. El entrar en cada imagen se explica cada una. La seguna imagen es causa de la mutación, que lleva a espontánea (errores al replicar el ADN) e inducida (por agentes físicos, químicos o biológicos). La tercera imagen es casos graves o algo así, y de divide en alelos letales (hablar de fibrosis quistica), y cáncer (que no siempre es letal). </t>
-  </si>
-  <si>
-    <t>Las enfermedades genéticas</t>
-  </si>
-  <si>
     <t>Interactivo que presenta diferentes enfermedades genéticas hereditarias y no hereditarias</t>
   </si>
   <si>
@@ -617,9 +611,6 @@
     <t>El ligamiento y el entrecruzamiento</t>
   </si>
   <si>
-    <t xml:space="preserve">La herencia ligada al sexo </t>
-  </si>
-  <si>
     <t>Análisis de pedigríes humanos</t>
   </si>
   <si>
@@ -665,9 +656,6 @@
     <t>Actividad para reforzar lo aprendido sobre la herencia ligada al sexo</t>
   </si>
   <si>
-    <t>Las diferentes formas de expresión de genes</t>
-  </si>
-  <si>
     <t>Recurso M1B-02</t>
   </si>
   <si>
@@ -699,6 +687,18 @@
   </si>
   <si>
     <t>Refuerza tu aprendizaje: El diagnóstico genético</t>
+  </si>
+  <si>
+    <t>Las diferentes formas de expresión de los genes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primera imagen del menú es "tipos de mutación", y lleva a imágenes que representan distontos tipos de mutación: somática, germinal, génica, cromosómica, genómica. El entrar en cada imagen se explica cada una. La seguna imagen es causa de la mutación, que lleva a espontánea (errores al replicar el ADN) e inducida (por agentes físicos, químicos o biológicos). La tercera imagen es casos graves o algo así, y de divide en alelos letales (hablar de fibrosis quistica), y cáncer (que no siempre es letal). </t>
+  </si>
+  <si>
+    <t>Las enfermedades genéticas hereditarias y no hereditarias</t>
+  </si>
+  <si>
+    <t>La herencia del sexo y de los caracteres que están en los cromosomas sexuales</t>
   </si>
 </sst>
 </file>
@@ -1617,7 +1617,7 @@
   <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1787,16 +1787,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="S3" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="T3" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="S3" s="22" t="s">
+      <c r="U3" s="23" t="s">
         <v>157</v>
-      </c>
-      <c r="T3" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="U3" s="23" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1846,16 +1846,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="57" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="S4" s="57" t="s">
+        <v>155</v>
+      </c>
+      <c r="T4" s="57" t="s">
+        <v>161</v>
+      </c>
+      <c r="U4" s="58" t="s">
         <v>157</v>
-      </c>
-      <c r="T4" s="57" t="s">
-        <v>163</v>
-      </c>
-      <c r="U4" s="58" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="F5" s="60"/>
       <c r="G5" s="62" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H5" s="30">
         <v>3</v>
@@ -1905,16 +1905,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="S5" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="T5" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="S5" s="11" t="s">
+      <c r="U5" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="T5" s="45" t="s">
-        <v>170</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1935,7 +1935,7 @@
       </c>
       <c r="F6" s="38"/>
       <c r="G6" s="40" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H6" s="30">
         <v>4</v>
@@ -1966,16 +1966,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="S6" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="T6" s="45" t="s">
+        <v>162</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="T6" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1996,7 +1996,7 @@
       </c>
       <c r="F7" s="38"/>
       <c r="G7" s="40" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H7" s="30">
         <v>5</v>
@@ -2020,19 +2020,19 @@
         <v>19</v>
       </c>
       <c r="Q7" s="47" t="s">
+        <v>183</v>
+      </c>
+      <c r="R7" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="S7" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="R7" s="27" t="s">
+      <c r="T7" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="U7" s="36" t="s">
         <v>186</v>
-      </c>
-      <c r="S7" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="T7" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="U7" s="36" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2053,7 +2053,7 @@
       </c>
       <c r="F8" s="38"/>
       <c r="G8" s="40" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="H8" s="30">
         <v>6</v>
@@ -2084,16 +2084,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="27" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="S8" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="T8" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="U8" s="36" t="s">
         <v>169</v>
-      </c>
-      <c r="T8" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="U8" s="36" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2114,7 +2114,7 @@
       </c>
       <c r="F9" s="38"/>
       <c r="G9" s="40" t="s">
-        <v>116</v>
+        <v>225</v>
       </c>
       <c r="H9" s="30">
         <v>7</v>
@@ -2138,19 +2138,19 @@
         <v>19</v>
       </c>
       <c r="Q9" s="47" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R9" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="S9" s="27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="T9" s="27" t="s">
         <v>116</v>
       </c>
       <c r="U9" s="36" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="F10" s="38"/>
       <c r="G10" s="40" t="s">
-        <v>198</v>
+        <v>117</v>
       </c>
       <c r="H10" s="30">
         <v>8</v>
@@ -2180,7 +2180,7 @@
         <v>92</v>
       </c>
       <c r="J10" s="41" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K10" s="43" t="s">
         <v>69</v>
@@ -2200,16 +2200,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="27" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="S10" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="T10" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="U10" s="36" t="s">
         <v>169</v>
-      </c>
-      <c r="T10" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="U10" s="36" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2230,7 +2230,7 @@
       </c>
       <c r="F11" s="38"/>
       <c r="G11" s="40" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="H11" s="30">
         <v>9</v>
@@ -2261,16 +2261,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="S11" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="T11" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="U11" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="T11" s="45" t="s">
-        <v>173</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2289,7 +2289,7 @@
       <c r="E12" s="29"/>
       <c r="F12" s="38"/>
       <c r="G12" s="40" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="H12" s="30">
         <v>10</v>
@@ -2320,16 +2320,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="S12" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="T12" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="U12" s="36" t="s">
         <v>157</v>
-      </c>
-      <c r="T12" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="U12" s="36" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2348,7 +2348,7 @@
       <c r="E13" s="29"/>
       <c r="F13" s="38"/>
       <c r="G13" s="40" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H13" s="30">
         <v>11</v>
@@ -2379,16 +2379,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="S13" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="T13" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="U13" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="T13" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2433,19 +2433,19 @@
         <v>19</v>
       </c>
       <c r="Q14" s="48" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R14" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="S14" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="T14" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="U14" s="37" t="s">
         <v>189</v>
-      </c>
-      <c r="T14" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="U14" s="37" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2462,11 +2462,11 @@
         <v>122</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F15" s="38"/>
       <c r="G15" s="40" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H15" s="30">
         <v>13</v>
@@ -2495,16 +2495,16 @@
         <v>6</v>
       </c>
       <c r="R15" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="S15" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="T15" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="U15" s="37" t="s">
         <v>169</v>
-      </c>
-      <c r="T15" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="U15" s="37" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2521,11 +2521,11 @@
         <v>122</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F16" s="38"/>
       <c r="G16" s="40" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H16" s="30">
         <v>14</v>
@@ -2554,16 +2554,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="S16" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="T16" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="U16" s="37" t="s">
         <v>169</v>
-      </c>
-      <c r="T16" s="28" t="s">
-        <v>177</v>
-      </c>
-      <c r="U16" s="37" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2584,7 +2584,7 @@
       </c>
       <c r="F17" s="38"/>
       <c r="G17" s="40" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="H17" s="30">
         <v>15</v>
@@ -2593,7 +2593,7 @@
         <v>92</v>
       </c>
       <c r="J17" s="41" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="K17" s="43" t="s">
         <v>69</v>
@@ -2613,16 +2613,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="S17" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="T17" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="U17" s="37" t="s">
         <v>169</v>
-      </c>
-      <c r="T17" s="28" t="s">
-        <v>174</v>
-      </c>
-      <c r="U17" s="37" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2639,11 +2639,11 @@
         <v>129</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F18" s="38"/>
       <c r="G18" s="40" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H18" s="30">
         <v>16</v>
@@ -2652,7 +2652,7 @@
         <v>91</v>
       </c>
       <c r="J18" s="41" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K18" s="43" t="s">
         <v>69</v>
@@ -2665,7 +2665,7 @@
       </c>
       <c r="N18" s="9"/>
       <c r="O18" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="P18" s="44" t="s">
         <v>19</v>
@@ -2674,16 +2674,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="S18" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="T18" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="U18" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="T18" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2700,7 +2700,7 @@
         <v>129</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F19" s="38"/>
       <c r="G19" s="40" t="s">
@@ -2733,16 +2733,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="S19" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="T19" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="U19" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="T19" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="U19" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2759,11 +2759,9 @@
         <v>129</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="F20" s="38" t="s">
-        <v>138</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="F20" s="38"/>
       <c r="G20" s="40" t="s">
         <v>133</v>
       </c>
@@ -2787,7 +2785,7 @@
       </c>
       <c r="N20" s="9"/>
       <c r="O20" s="8" t="s">
-        <v>135</v>
+        <v>223</v>
       </c>
       <c r="P20" s="44" t="s">
         <v>19</v>
@@ -2796,16 +2794,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="S20" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="T20" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="U20" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="T20" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2822,13 +2820,11 @@
         <v>129</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="F21" s="38" t="s">
-        <v>138</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="F21" s="38"/>
       <c r="G21" s="40" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="H21" s="30">
         <v>19</v>
@@ -2837,7 +2833,7 @@
         <v>92</v>
       </c>
       <c r="J21" s="41" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="K21" s="43" t="s">
         <v>69</v>
@@ -2857,16 +2853,16 @@
         <v>6</v>
       </c>
       <c r="R21" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="S21" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="T21" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="U21" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="T21" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2883,13 +2879,13 @@
         <v>129</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F22" s="38" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G22" s="40" t="s">
-        <v>136</v>
+        <v>224</v>
       </c>
       <c r="H22" s="30">
         <v>20</v>
@@ -2898,7 +2894,7 @@
         <v>91</v>
       </c>
       <c r="J22" s="41" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K22" s="43" t="s">
         <v>69</v>
@@ -2918,16 +2914,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="S22" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="T22" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="U22" s="37" t="s">
         <v>157</v>
-      </c>
-      <c r="T22" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="U22" s="37" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2948,7 +2944,7 @@
       </c>
       <c r="F23" s="38"/>
       <c r="G23" s="40" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="H23" s="30">
         <v>21</v>
@@ -2957,7 +2953,7 @@
         <v>92</v>
       </c>
       <c r="J23" s="41" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K23" s="43" t="s">
         <v>69</v>
@@ -2977,16 +2973,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="S23" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="T23" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="U23" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="T23" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="U23" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3000,12 +2996,12 @@
         <v>98</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E24" s="29"/>
       <c r="F24" s="38"/>
       <c r="G24" s="40" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H24" s="30">
         <v>22</v>
@@ -3014,7 +3010,7 @@
         <v>91</v>
       </c>
       <c r="J24" s="41" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K24" s="43" t="s">
         <v>69</v>
@@ -3027,7 +3023,7 @@
       </c>
       <c r="N24" s="9"/>
       <c r="O24" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P24" s="44" t="s">
         <v>19</v>
@@ -3036,16 +3032,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="S24" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="T24" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="U24" s="37" t="s">
         <v>157</v>
-      </c>
-      <c r="T24" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="U24" s="37" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3059,14 +3055,14 @@
         <v>98</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F25" s="38"/>
       <c r="G25" s="40" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H25" s="30">
         <v>23</v>
@@ -3075,7 +3071,7 @@
         <v>91</v>
       </c>
       <c r="J25" s="41" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K25" s="43" t="s">
         <v>70</v>
@@ -3090,19 +3086,19 @@
         <v>19</v>
       </c>
       <c r="Q25" s="48" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R25" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="S25" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="T25" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="U25" s="37" t="s">
         <v>189</v>
-      </c>
-      <c r="T25" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="U25" s="37" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3116,14 +3112,14 @@
         <v>98</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F26" s="38"/>
       <c r="G26" s="40" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="H26" s="30">
         <v>24</v>
@@ -3132,7 +3128,7 @@
         <v>92</v>
       </c>
       <c r="J26" s="41" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K26" s="43" t="s">
         <v>69</v>
@@ -3152,16 +3148,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="S26" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="T26" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="U26" s="37" t="s">
         <v>169</v>
-      </c>
-      <c r="T26" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="U26" s="37" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3175,14 +3171,14 @@
         <v>98</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F27" s="38"/>
       <c r="G27" s="41" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H27" s="30">
         <v>25</v>
@@ -3191,7 +3187,7 @@
         <v>92</v>
       </c>
       <c r="J27" s="41" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="K27" s="43" t="s">
         <v>69</v>
@@ -3211,16 +3207,16 @@
         <v>6</v>
       </c>
       <c r="R27" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="S27" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="T27" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="U27" s="37" t="s">
         <v>169</v>
-      </c>
-      <c r="T27" s="28" t="s">
-        <v>215</v>
-      </c>
-      <c r="U27" s="37" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3234,14 +3230,14 @@
         <v>98</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>93</v>
       </c>
       <c r="F28" s="38"/>
       <c r="G28" s="40" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="H28" s="30">
         <v>26</v>
@@ -3250,7 +3246,7 @@
         <v>92</v>
       </c>
       <c r="J28" s="41" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K28" s="43" t="s">
         <v>69</v>
@@ -3263,7 +3259,7 @@
         <v>62</v>
       </c>
       <c r="O28" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="P28" s="44" t="s">
         <v>19</v>
@@ -3272,16 +3268,16 @@
         <v>6</v>
       </c>
       <c r="R28" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="S28" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="T28" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="U28" s="37" t="s">
         <v>169</v>
-      </c>
-      <c r="T28" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="U28" s="37" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3300,7 +3296,7 @@
       <c r="E29" s="29"/>
       <c r="F29" s="38"/>
       <c r="G29" s="40" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H29" s="30">
         <v>27</v>
@@ -3309,7 +3305,7 @@
         <v>92</v>
       </c>
       <c r="J29" s="41" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K29" s="43" t="s">
         <v>70</v>
@@ -3324,19 +3320,19 @@
         <v>19</v>
       </c>
       <c r="Q29" s="48" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R29" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="S29" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="T29" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="U29" s="37" t="s">
         <v>189</v>
-      </c>
-      <c r="T29" s="28" t="s">
-        <v>193</v>
-      </c>
-      <c r="U29" s="37" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3355,7 +3351,7 @@
       <c r="E30" s="29"/>
       <c r="F30" s="38"/>
       <c r="G30" s="40" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H30" s="30">
         <v>28</v>
@@ -3364,7 +3360,7 @@
         <v>92</v>
       </c>
       <c r="J30" s="41" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K30" s="43" t="s">
         <v>69</v>
@@ -3384,16 +3380,16 @@
         <v>6</v>
       </c>
       <c r="R30" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="S30" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="T30" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="U30" s="37" t="s">
         <v>169</v>
-      </c>
-      <c r="T30" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="U30" s="37" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3412,7 +3408,7 @@
       <c r="E31" s="29"/>
       <c r="F31" s="38"/>
       <c r="G31" s="40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H31" s="30">
         <v>29</v>
@@ -3421,7 +3417,7 @@
         <v>92</v>
       </c>
       <c r="J31" s="41" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K31" s="43" t="s">
         <v>69</v>
@@ -3441,16 +3437,16 @@
         <v>6</v>
       </c>
       <c r="R31" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="S31" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="T31" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="U31" s="37" t="s">
         <v>169</v>
-      </c>
-      <c r="T31" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="U31" s="37" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3469,7 +3465,7 @@
       <c r="E32" s="29"/>
       <c r="F32" s="38"/>
       <c r="G32" s="40" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="H32" s="30">
         <v>30</v>
@@ -3478,13 +3474,13 @@
         <v>92</v>
       </c>
       <c r="J32" s="41" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K32" s="43" t="s">
         <v>69</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="M32" s="9"/>
       <c r="N32" s="9"/>
@@ -3523,7 +3519,7 @@
         <v>92</v>
       </c>
       <c r="J33" s="41" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K33" s="43" t="s">
         <v>69</v>
@@ -3543,16 +3539,16 @@
         <v>6</v>
       </c>
       <c r="R33" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="S33" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="T33" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="U33" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="T33" s="45" t="s">
-        <v>182</v>
-      </c>
-      <c r="U33" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -3571,7 +3567,7 @@
       <c r="E34" s="29"/>
       <c r="F34" s="38"/>
       <c r="G34" s="40" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H34" s="30">
         <v>32</v>
@@ -3580,7 +3576,7 @@
         <v>92</v>
       </c>
       <c r="J34" s="41" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K34" s="43" t="s">
         <v>69</v>
@@ -3600,16 +3596,16 @@
         <v>6</v>
       </c>
       <c r="R34" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="S34" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="T34" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="U34" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="T34" s="45" t="s">
-        <v>181</v>
-      </c>
-      <c r="U34" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrección nombres de recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion07/ESCALETA_CN_08_07_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion07/ESCALETA_CN_08_07_CO.xlsx
@@ -1,25 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mpgarcia\Desktop\CienciasNaturales\fuentes\contenidos\grado08\guion07\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="9240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="ESCALETA" sheetId="1" r:id="rId1"/>
     <sheet name="DATOS" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="VER" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ESCALETA!$A$1:$U$34</definedName>
-  </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="226">
   <si>
     <t>Asignatura</t>
   </si>
@@ -340,9 +332,6 @@
     <t>La teoría cromosómica de la herencia: Mendel, Sutton y Boveri</t>
   </si>
   <si>
-    <t>Actividad para repasar los aportes hechos a la genética por Mendel, Sutton y Boveri</t>
-  </si>
-  <si>
     <t>Hay una ficha para cada investigador. En la parte de Mendel se deben explicar sus leyes de la herencia.</t>
   </si>
   <si>
@@ -352,9 +341,6 @@
     <t>Los aportes de Morgan a la genética</t>
   </si>
   <si>
-    <t>Interactivo que expone la teoría cromosómica de la herencia a partir de los trabajos de Mendel, Sutton y Boveri. Se deben mencionar algunos datos históricos (con qué organismo trabajaron, cuándo, en dónde), y se deben explicar las leyes de Mendel, recordando que esto es algo que los estudiantes ya vieron, por lo que sólo se necesita hacer el recordatorio.</t>
-  </si>
-  <si>
     <t>Interactivo que presenta los experimentos y aportes de Thomas Morgan</t>
   </si>
   <si>
@@ -364,9 +350,6 @@
     <t>Dos imágenes de menú, una para ligamiento y otra para entrecruzamiento. En la explicación de este último se debe resaltar la influencia de este proceso en la variabilidad genpetica, y recordar por qué esta es importante (los estudiantes ya lo deben haber visto)</t>
   </si>
   <si>
-    <t xml:space="preserve">Interactivo que explica los fenómenos de ligamiento y entrecruzamiento. Explicar que el entrecruzamiento es una forma de recombinación genética (y explicar qué es recombinación), y qué es el quiasma. </t>
-  </si>
-  <si>
     <t>Actividad para repasar algunos aspectos relacionados con la variabilidad genética</t>
   </si>
   <si>
@@ -421,9 +404,6 @@
     <t xml:space="preserve">Las enfermedades genéticas </t>
   </si>
   <si>
-    <t xml:space="preserve">Se hacen árboles genealógicos que muestran distintas condiciones con diferentes patrones de herencia. Al comienzo sale una parte del árbol, y al avanzar en el recurso se va revelando el resto. Hay un formato hecho para esto, que puede adaptarse; preguntarlo. </t>
-  </si>
-  <si>
     <t>Identifica los tipos de enfermedades genéticas</t>
   </si>
   <si>
@@ -634,9 +614,6 @@
     <t>Interactivo que presenta los diferentes tipos de enfermedades genéticas</t>
   </si>
   <si>
-    <t>Clasificación de las enfermedades genéticas</t>
-  </si>
-  <si>
     <t xml:space="preserve">Exponer las enfermedades monogénicas, multifactoriales, cromosómicas, mitocondriales. Se debe hacer una ficha para diferenciar enfermedades genéticas hereditarias y no hereditarias; puede ser la última, y allí se explixca que en las otras categorías puede haber enfermedades que se hereden y otras que no. Por ejemplo, las monogénicas pueden ser mutaciones en el cromosoma X o en un cromosoma somático (no hay que olvidar que no se conocen enfermedades ligadas a Y). Esta ficha debe ser diferente de alguna forma, para que esta separación no parezca de la misma categoría que las anteriores. Se puede, por ejemplo, poner como título de las demás fichas una palabra o frase (Enfermedades monogénicas, p.e.), y en la última una pregunta: "¿Son hereditarias o no?", o alguna cosa así.  </t>
   </si>
   <si>
@@ -655,9 +632,6 @@
     <t>MAPA CONCEPTUAL</t>
   </si>
   <si>
-    <t>Repasa los aportes a la genética de Mendel, Sutton y Boveri</t>
-  </si>
-  <si>
     <t>Actividad para reforzar lo aprendido sobre la herencia ligada al sexo</t>
   </si>
   <si>
@@ -694,22 +668,37 @@
     <t>Refuerza tu aprendizaje: El diagnóstico genético</t>
   </si>
   <si>
-    <t>Las diferentes formas de expresión de los genes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Primera imagen del menú es "tipos de mutación", y lleva a imágenes que representan distontos tipos de mutación: somática, germinal, génica, cromosómica, genómica. El entrar en cada imagen se explica cada una. La seguna imagen es causa de la mutación, que lleva a espontánea (errores al replicar el ADN) e inducida (por agentes físicos, químicos o biológicos). La tercera imagen es casos graves o algo así, y de divide en alelos letales (hablar de fibrosis quistica), y cáncer (que no siempre es letal). </t>
   </si>
   <si>
     <t>Las enfermedades genéticas hereditarias y no hereditarias</t>
   </si>
   <si>
-    <t>La herencia del sexo y de los caracteres que están en los cromosomas sexuales</t>
-  </si>
-  <si>
     <t>Recurso M1C-01</t>
   </si>
   <si>
-    <t>Recurso M102AB-02</t>
+    <t>Se hacen árboles genealógicos que muestran distintas condiciones con diferentes patrones de herencia. Al comienzo sale una parte del árbol, y al avanzar en el recurso se va revelando el resto. Hay un formato hecho para esto, que puede adaptarse; preguntarlo.</t>
+  </si>
+  <si>
+    <t>Las formas de herencia y expresión de los genes</t>
+  </si>
+  <si>
+    <t>Los descubrimientos de Mendel, Sutton, Boveri y Morgan</t>
+  </si>
+  <si>
+    <t>Actividad para repasar los aportes hechos a la genética por Mendel, Sutton, Boveri y Morgan</t>
+  </si>
+  <si>
+    <t>La herencia del sexo y de los caracteres en los cromosomas sexuales</t>
+  </si>
+  <si>
+    <t>Interactivo que expone la teoría cromosómica de la herencia a partir de los trabajos de Mendel, Sutton y Boveri.</t>
+  </si>
+  <si>
+    <t>Interactivo que explica los fenómenos de ligamiento y entrecruzamiento.</t>
+  </si>
+  <si>
+    <t>La clasificación de las enfermedades genéticas</t>
   </si>
 </sst>
 </file>
@@ -1617,7 +1606,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1627,8 +1616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,14 +1634,14 @@
     <col min="10" max="10" width="129.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" style="25" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" style="25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" style="10" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" style="25" customWidth="1"/>
-    <col min="15" max="15" width="4.140625" style="26" customWidth="1"/>
-    <col min="16" max="16" width="5.85546875" style="24" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="14" style="25" customWidth="1"/>
+    <col min="15" max="15" width="90.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" style="24" customWidth="1"/>
     <col min="17" max="17" width="9.140625" style="10" customWidth="1"/>
     <col min="18" max="18" width="11.140625" style="10" customWidth="1"/>
-    <col min="19" max="19" width="15.42578125" style="10" customWidth="1"/>
-    <col min="20" max="20" width="37.85546875" style="10" customWidth="1"/>
+    <col min="19" max="19" width="44.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="60.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="18.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="11.42578125" style="10"/>
   </cols>
@@ -1776,7 +1765,7 @@
         <v>91</v>
       </c>
       <c r="J3" s="39" t="s">
-        <v>107</v>
+        <v>223</v>
       </c>
       <c r="K3" s="42" t="s">
         <v>69</v>
@@ -1789,7 +1778,7 @@
       </c>
       <c r="N3" s="20"/>
       <c r="O3" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P3" s="46" t="s">
         <v>19</v>
@@ -1798,16 +1787,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="22" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="S3" s="22" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="T3" s="22" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="U3" s="23" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1824,11 +1813,11 @@
         <v>99</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F4" s="38"/>
       <c r="G4" s="64" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H4" s="30">
         <v>2</v>
@@ -1837,7 +1826,7 @@
         <v>91</v>
       </c>
       <c r="J4" s="51" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K4" s="52" t="s">
         <v>69</v>
@@ -1857,16 +1846,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="57" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="S4" s="57" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="T4" s="57" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="U4" s="58" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1883,11 +1872,11 @@
         <v>99</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F5" s="60"/>
       <c r="G5" s="62" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="H5" s="30">
         <v>3</v>
@@ -1896,7 +1885,7 @@
         <v>92</v>
       </c>
       <c r="J5" s="41" t="s">
-        <v>103</v>
+        <v>221</v>
       </c>
       <c r="K5" s="43" t="s">
         <v>69</v>
@@ -1916,16 +1905,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="T5" s="45" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1942,11 +1931,11 @@
         <v>99</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F6" s="38"/>
       <c r="G6" s="40" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H6" s="30">
         <v>4</v>
@@ -1955,7 +1944,7 @@
         <v>91</v>
       </c>
       <c r="J6" s="41" t="s">
-        <v>111</v>
+        <v>224</v>
       </c>
       <c r="K6" s="43" t="s">
         <v>69</v>
@@ -1968,7 +1957,7 @@
       </c>
       <c r="N6" s="9"/>
       <c r="O6" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P6" s="44" t="s">
         <v>19</v>
@@ -1977,16 +1966,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="T6" s="45" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2003,11 +1992,11 @@
         <v>99</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F7" s="38"/>
       <c r="G7" s="40" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H7" s="30">
         <v>5</v>
@@ -2016,7 +2005,7 @@
         <v>92</v>
       </c>
       <c r="J7" s="41" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K7" s="43" t="s">
         <v>70</v>
@@ -2031,19 +2020,19 @@
         <v>19</v>
       </c>
       <c r="Q7" s="47" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="R7" s="27" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="S7" s="27" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="T7" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="U7" s="36" t="s">
         <v>182</v>
-      </c>
-      <c r="U7" s="36" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2064,7 +2053,7 @@
       </c>
       <c r="F8" s="38"/>
       <c r="G8" s="40" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="H8" s="30">
         <v>6</v>
@@ -2073,7 +2062,7 @@
         <v>92</v>
       </c>
       <c r="J8" s="41" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K8" s="43" t="s">
         <v>69</v>
@@ -2086,7 +2075,7 @@
         <v>62</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="P8" s="44" t="s">
         <v>19</v>
@@ -2095,16 +2084,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="S8" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="T8" s="27" t="s">
         <v>166</v>
       </c>
-      <c r="S8" s="27" t="s">
-        <v>167</v>
-      </c>
-      <c r="T8" s="27" t="s">
-        <v>170</v>
-      </c>
       <c r="U8" s="36" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2118,14 +2107,14 @@
         <v>98</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F9" s="38"/>
       <c r="G9" s="40" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H9" s="30">
         <v>7</v>
@@ -2134,7 +2123,7 @@
         <v>91</v>
       </c>
       <c r="J9" s="41" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K9" s="43" t="s">
         <v>70</v>
@@ -2149,19 +2138,19 @@
         <v>19</v>
       </c>
       <c r="Q9" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="R9" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="S9" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="R9" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="S9" s="27" t="s">
-        <v>187</v>
-      </c>
       <c r="T9" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="U9" s="36" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2175,14 +2164,14 @@
         <v>98</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F10" s="38"/>
       <c r="G10" s="40" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H10" s="30">
         <v>8</v>
@@ -2191,7 +2180,7 @@
         <v>92</v>
       </c>
       <c r="J10" s="41" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="K10" s="43" t="s">
         <v>69</v>
@@ -2211,16 +2200,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="27" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="S10" s="27" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="T10" s="27" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="U10" s="36" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2234,14 +2223,14 @@
         <v>98</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E11" s="29" t="s">
         <v>93</v>
       </c>
       <c r="F11" s="38"/>
       <c r="G11" s="40" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="H11" s="30">
         <v>9</v>
@@ -2250,7 +2239,7 @@
         <v>92</v>
       </c>
       <c r="J11" s="41" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="K11" s="43" t="s">
         <v>69</v>
@@ -2263,7 +2252,7 @@
         <v>62</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="P11" s="44" t="s">
         <v>19</v>
@@ -2272,16 +2261,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="S11" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="T11" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="T11" s="45" t="s">
-        <v>171</v>
-      </c>
       <c r="U11" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2295,12 +2284,12 @@
         <v>98</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E12" s="29"/>
       <c r="F12" s="38"/>
       <c r="G12" s="40" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H12" s="30">
         <v>10</v>
@@ -2309,7 +2298,7 @@
         <v>91</v>
       </c>
       <c r="J12" s="41" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="K12" s="43" t="s">
         <v>69</v>
@@ -2322,7 +2311,7 @@
       </c>
       <c r="N12" s="9"/>
       <c r="O12" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="P12" s="44" t="s">
         <v>19</v>
@@ -2331,16 +2320,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="S12" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="T12" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="S12" s="27" t="s">
-        <v>155</v>
-      </c>
-      <c r="T12" s="27" t="s">
-        <v>158</v>
-      </c>
       <c r="U12" s="36" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2354,12 +2343,12 @@
         <v>98</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E13" s="29"/>
       <c r="F13" s="38"/>
       <c r="G13" s="40" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H13" s="30">
         <v>11</v>
@@ -2368,7 +2357,7 @@
         <v>91</v>
       </c>
       <c r="J13" s="41" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="K13" s="43" t="s">
         <v>69</v>
@@ -2381,7 +2370,7 @@
       </c>
       <c r="N13" s="9"/>
       <c r="O13" s="8" t="s">
-        <v>130</v>
+        <v>218</v>
       </c>
       <c r="P13" s="44" t="s">
         <v>19</v>
@@ -2390,16 +2379,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="S13" s="11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="T13" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2413,14 +2402,14 @@
         <v>98</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F14" s="38"/>
       <c r="G14" s="40" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H14" s="30">
         <v>12</v>
@@ -2429,7 +2418,7 @@
         <v>92</v>
       </c>
       <c r="J14" s="41" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K14" s="43" t="s">
         <v>70</v>
@@ -2444,19 +2433,19 @@
         <v>19</v>
       </c>
       <c r="Q14" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="R14" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="S14" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="R14" s="28" t="s">
+      <c r="T14" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="S14" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="T14" s="28" t="s">
-        <v>188</v>
-      </c>
       <c r="U14" s="37" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2470,14 +2459,14 @@
         <v>98</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F15" s="38"/>
       <c r="G15" s="40" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H15" s="30">
         <v>13</v>
@@ -2486,7 +2475,7 @@
         <v>92</v>
       </c>
       <c r="J15" s="41" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="K15" s="43" t="s">
         <v>69</v>
@@ -2506,16 +2495,16 @@
         <v>6</v>
       </c>
       <c r="R15" s="28" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="S15" s="28" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="T15" s="28" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="U15" s="37" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2529,14 +2518,14 @@
         <v>98</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F16" s="38"/>
       <c r="G16" s="40" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="H16" s="30">
         <v>14</v>
@@ -2545,7 +2534,7 @@
         <v>92</v>
       </c>
       <c r="J16" s="41" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K16" s="43" t="s">
         <v>69</v>
@@ -2565,16 +2554,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="28" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="S16" s="28" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="T16" s="28" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="U16" s="37" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2588,14 +2577,14 @@
         <v>98</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E17" s="29" t="s">
         <v>93</v>
       </c>
       <c r="F17" s="38"/>
       <c r="G17" s="40" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="H17" s="30">
         <v>15</v>
@@ -2604,7 +2593,7 @@
         <v>92</v>
       </c>
       <c r="J17" s="41" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="K17" s="43" t="s">
         <v>69</v>
@@ -2624,16 +2613,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="28" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="S17" s="28" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="T17" s="28" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="U17" s="37" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2647,14 +2636,14 @@
         <v>98</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F18" s="38"/>
       <c r="G18" s="40" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="H18" s="30">
         <v>16</v>
@@ -2663,7 +2652,7 @@
         <v>91</v>
       </c>
       <c r="J18" s="41" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="K18" s="43" t="s">
         <v>69</v>
@@ -2676,7 +2665,7 @@
       </c>
       <c r="N18" s="9"/>
       <c r="O18" s="8" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="P18" s="44" t="s">
         <v>19</v>
@@ -2685,16 +2674,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="S18" s="11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="T18" s="11" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2708,14 +2697,14 @@
         <v>98</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F19" s="38"/>
       <c r="G19" s="40" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H19" s="30">
         <v>17</v>
@@ -2724,7 +2713,7 @@
         <v>92</v>
       </c>
       <c r="J19" s="41" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="K19" s="43" t="s">
         <v>69</v>
@@ -2744,16 +2733,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="S19" s="11" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="T19" s="11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2767,14 +2756,14 @@
         <v>98</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F20" s="38"/>
       <c r="G20" s="40" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H20" s="30">
         <v>18</v>
@@ -2783,7 +2772,7 @@
         <v>91</v>
       </c>
       <c r="J20" s="41" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="K20" s="43" t="s">
         <v>69</v>
@@ -2796,7 +2785,7 @@
       </c>
       <c r="N20" s="9"/>
       <c r="O20" s="8" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="P20" s="44" t="s">
         <v>19</v>
@@ -2805,16 +2794,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="S20" s="11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="T20" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2828,14 +2817,14 @@
         <v>98</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F21" s="38"/>
       <c r="G21" s="40" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="H21" s="30">
         <v>19</v>
@@ -2844,7 +2833,7 @@
         <v>92</v>
       </c>
       <c r="J21" s="41" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="K21" s="43" t="s">
         <v>69</v>
@@ -2864,16 +2853,16 @@
         <v>6</v>
       </c>
       <c r="R21" s="11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="S21" s="11" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="T21" s="11" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2887,16 +2876,16 @@
         <v>98</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F22" s="38" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G22" s="40" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="H22" s="30">
         <v>20</v>
@@ -2905,7 +2894,7 @@
         <v>91</v>
       </c>
       <c r="J22" s="41" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="K22" s="43" t="s">
         <v>69</v>
@@ -2925,16 +2914,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="28" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="S22" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="T22" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="T22" s="28" t="s">
-        <v>159</v>
-      </c>
       <c r="U22" s="37" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2948,14 +2937,14 @@
         <v>98</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E23" s="29" t="s">
         <v>93</v>
       </c>
       <c r="F23" s="38"/>
       <c r="G23" s="40" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="H23" s="30">
         <v>21</v>
@@ -2964,7 +2953,7 @@
         <v>92</v>
       </c>
       <c r="J23" s="41" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K23" s="43" t="s">
         <v>69</v>
@@ -2984,16 +2973,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="S23" s="11" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="T23" s="11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3007,12 +2996,12 @@
         <v>98</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E24" s="29"/>
       <c r="F24" s="38"/>
       <c r="G24" s="40" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H24" s="30">
         <v>22</v>
@@ -3021,7 +3010,7 @@
         <v>91</v>
       </c>
       <c r="J24" s="41" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K24" s="43" t="s">
         <v>69</v>
@@ -3034,7 +3023,7 @@
       </c>
       <c r="N24" s="9"/>
       <c r="O24" s="8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="P24" s="44" t="s">
         <v>19</v>
@@ -3043,16 +3032,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="28" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="S24" s="28" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="T24" s="28" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="U24" s="37" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3066,14 +3055,14 @@
         <v>98</v>
       </c>
       <c r="D25" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" s="29" t="s">
         <v>139</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>143</v>
       </c>
       <c r="F25" s="38"/>
       <c r="G25" s="40" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H25" s="30">
         <v>23</v>
@@ -3082,7 +3071,7 @@
         <v>91</v>
       </c>
       <c r="J25" s="41" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="K25" s="43" t="s">
         <v>70</v>
@@ -3097,19 +3086,19 @@
         <v>19</v>
       </c>
       <c r="Q25" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="R25" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="S25" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="R25" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="S25" s="28" t="s">
-        <v>187</v>
-      </c>
       <c r="T25" s="28" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="U25" s="37" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3123,14 +3112,14 @@
         <v>98</v>
       </c>
       <c r="D26" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" s="29" t="s">
         <v>139</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>143</v>
       </c>
       <c r="F26" s="38"/>
       <c r="G26" s="40" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="H26" s="30">
         <v>24</v>
@@ -3139,7 +3128,7 @@
         <v>92</v>
       </c>
       <c r="J26" s="41" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K26" s="43" t="s">
         <v>69</v>
@@ -3159,16 +3148,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="28" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="S26" s="28" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="T26" s="28" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="U26" s="37" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3182,14 +3171,14 @@
         <v>98</v>
       </c>
       <c r="D27" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" s="29" t="s">
         <v>139</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>143</v>
       </c>
       <c r="F27" s="38"/>
       <c r="G27" s="41" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H27" s="30">
         <v>25</v>
@@ -3198,7 +3187,7 @@
         <v>92</v>
       </c>
       <c r="J27" s="41" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="K27" s="43" t="s">
         <v>69</v>
@@ -3218,16 +3207,16 @@
         <v>6</v>
       </c>
       <c r="R27" s="28" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="S27" s="28" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="T27" s="28" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="U27" s="37" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3241,14 +3230,14 @@
         <v>98</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>93</v>
       </c>
       <c r="F28" s="38"/>
       <c r="G28" s="40" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="H28" s="30">
         <v>26</v>
@@ -3257,7 +3246,7 @@
         <v>92</v>
       </c>
       <c r="J28" s="41" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="K28" s="43" t="s">
         <v>69</v>
@@ -3270,7 +3259,7 @@
         <v>62</v>
       </c>
       <c r="O28" s="8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="P28" s="44" t="s">
         <v>19</v>
@@ -3279,16 +3268,16 @@
         <v>6</v>
       </c>
       <c r="R28" s="28" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="S28" s="28" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="T28" s="28" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="U28" s="37" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3307,7 +3296,7 @@
       <c r="E29" s="29"/>
       <c r="F29" s="38"/>
       <c r="G29" s="40" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H29" s="30">
         <v>27</v>
@@ -3316,7 +3305,7 @@
         <v>92</v>
       </c>
       <c r="J29" s="41" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="K29" s="43" t="s">
         <v>70</v>
@@ -3331,19 +3320,19 @@
         <v>19</v>
       </c>
       <c r="Q29" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="R29" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="S29" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="R29" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="S29" s="28" t="s">
-        <v>187</v>
-      </c>
       <c r="T29" s="28" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="U29" s="37" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3362,7 +3351,7 @@
       <c r="E30" s="29"/>
       <c r="F30" s="38"/>
       <c r="G30" s="40" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H30" s="30">
         <v>28</v>
@@ -3371,7 +3360,7 @@
         <v>92</v>
       </c>
       <c r="J30" s="41" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="K30" s="43" t="s">
         <v>69</v>
@@ -3391,16 +3380,16 @@
         <v>6</v>
       </c>
       <c r="R30" s="28" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="S30" s="28" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="T30" s="28" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="U30" s="37" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3419,7 +3408,7 @@
       <c r="E31" s="29"/>
       <c r="F31" s="38"/>
       <c r="G31" s="40" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H31" s="30">
         <v>29</v>
@@ -3428,7 +3417,7 @@
         <v>92</v>
       </c>
       <c r="J31" s="41" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K31" s="43" t="s">
         <v>69</v>
@@ -3448,16 +3437,16 @@
         <v>6</v>
       </c>
       <c r="R31" s="28" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="S31" s="28" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="T31" s="28" t="s">
-        <v>226</v>
+        <v>177</v>
       </c>
       <c r="U31" s="37" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3476,7 +3465,7 @@
       <c r="E32" s="29"/>
       <c r="F32" s="38"/>
       <c r="G32" s="40" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="H32" s="30">
         <v>30</v>
@@ -3485,13 +3474,13 @@
         <v>92</v>
       </c>
       <c r="J32" s="41" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="K32" s="43" t="s">
         <v>69</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="M32" s="9"/>
       <c r="N32" s="9"/>
@@ -3530,7 +3519,7 @@
         <v>92</v>
       </c>
       <c r="J33" s="41" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K33" s="43" t="s">
         <v>69</v>
@@ -3550,16 +3539,16 @@
         <v>6</v>
       </c>
       <c r="R33" s="11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="S33" s="11" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="T33" s="45" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="U33" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -3578,7 +3567,7 @@
       <c r="E34" s="29"/>
       <c r="F34" s="38"/>
       <c r="G34" s="40" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H34" s="30">
         <v>32</v>
@@ -3587,7 +3576,7 @@
         <v>92</v>
       </c>
       <c r="J34" s="41" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="K34" s="43" t="s">
         <v>69</v>
@@ -3607,23 +3596,25 @@
         <v>6</v>
       </c>
       <c r="R34" s="11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="S34" s="11" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="T34" s="45" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="U34" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U34">
-    <filterColumn colId="12" showButton="0"/>
-  </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -3639,11 +3630,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>